<commit_message>
Add MASE measurement to GA
</commit_message>
<xml_diff>
--- a/data/Benchmarks.xlsx
+++ b/data/Benchmarks.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\Master\dynamic-factor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\Master\dynamic-factor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921AD19-23E1-44D4-9FD5-0CCD149F944D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA80F6C-DF30-4925-9995-1C369FD078D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="4" r:id="rId1"/>
-    <sheet name="VAR" sheetId="6" r:id="rId2"/>
+    <sheet name="Salmon" sheetId="6" r:id="rId2"/>
     <sheet name="Oil" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="152">
   <si>
     <t>Maize</t>
   </si>
@@ -34673,8 +34673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD170B7-5247-4632-9345-E92016084A21}">
   <dimension ref="A1:U103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -34706,15 +34706,13 @@
       </c>
       <c r="C1" s="9">
         <f>COUNTIF($F$2:$AJ$100, A1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1"/>
       <c r="F1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -34745,9 +34743,7 @@
       <c r="F2" s="15">
         <v>40</v>
       </c>
-      <c r="G2" s="15">
-        <v>40</v>
-      </c>
+      <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -34776,7 +34772,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="7">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -34800,11 +34796,11 @@
       </c>
       <c r="C4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1"/>
       <c r="F4" s="7">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -35435,7 +35431,7 @@
       </c>
       <c r="C40" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1"/>
       <c r="G40" s="7"/>
@@ -36278,7 +36274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616A4956-0250-408C-BA81-1A0CBE7DF20B}">
   <dimension ref="A1:U103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -36340,7 +36336,7 @@
         <v>128</v>
       </c>
       <c r="C2" s="9">
-        <f t="shared" ref="C2:C65" si="0">COUNTIF($F$2:$AJ$100, A2)</f>
+        <f t="shared" ref="C2:C25" si="0">COUNTIF($F$2:$AJ$100, A2)</f>
         <v>0</v>
       </c>
       <c r="D2" s="13"/>

</xml_diff>